<commit_message>
Pert, motors i entrega perlin
</commit_message>
<xml_diff>
--- a/2n/Game Design/PERT projecte.xlsx
+++ b/2n/Game Design/PERT projecte.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FP\2n\Game Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D868EB5-CE51-407F-8D38-9701B824CF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="21705"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPM" sheetId="3" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <definedName name="vertex42_id" hidden="1">"critical-path-method.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Critical Path Method Spreadsheet"</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,13 +41,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Marc Albareda</author>
     <author>Vertex42</author>
   </authors>
   <commentList>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="1" shapeId="0">
+    <comment ref="A8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="1" shapeId="0">
+    <comment ref="B8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="1" shapeId="0">
+    <comment ref="C8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -154,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="1" shapeId="0">
+    <comment ref="I8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -197,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="1" shapeId="0">
+    <comment ref="J8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -221,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K8" authorId="1" shapeId="0">
+    <comment ref="K8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -264,7 +265,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="1" shapeId="0">
+    <comment ref="L8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -291,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M8" authorId="1" shapeId="0">
+    <comment ref="M8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -316,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="1" shapeId="0">
+    <comment ref="N8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -342,7 +343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="1" shapeId="0">
+    <comment ref="O8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -367,7 +368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="1" shapeId="0">
+    <comment ref="P8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -391,7 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q8" authorId="1" shapeId="0">
+    <comment ref="Q8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -426,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -439,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -464,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B62" authorId="0" shapeId="0">
+    <comment ref="B62" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -741,7 +742,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1372,48 +1373,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="36" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="20% - Èmfasi1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Èmfasi2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Èmfasi3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Èmfasi4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Èmfasi5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Èmfasi6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Èmfasi1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Èmfasi2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Èmfasi3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Èmfasi4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Èmfasi5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Èmfasi6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Èmfasi1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Èmfasi2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Èmfasi3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Èmfasi4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Èmfasi5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Èmfasi6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bé" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Càlcul" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cel·la de comprovació" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Cel·la enllaçada" xfId="36" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Èmfasi1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Èmfasi2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Èmfasi3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Èmfasi4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Èmfasi5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Èmfasi6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Enllaç" xfId="34" builtinId="8"/>
     <cellStyle name="Entrada" xfId="35" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="34" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Incorrecte" xfId="25" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="37" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="38" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="39" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="42" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="40" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="38" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Resultat" xfId="39" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Text d'advertiment" xfId="42" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Text explicatiu" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Títol" xfId="40" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Títol 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Títol 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Títol 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Títol 4" xfId="33" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="3">
@@ -1530,7 +1531,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="ca-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1711,7 +1712,7 @@
                   <c:v>-0.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.75</c:v>
+                  <c:v>13.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1741,61 +1742,61 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29.75</c:v>
+                  <c:v>27.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>21</c:v>
-                </c:pt>
                 <c:pt idx="14">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>25</c:v>
-                </c:pt>
                 <c:pt idx="20">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>27.75</c:v>
+                  <c:v>26.75</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>44.75</c:v>
+                  <c:v>39.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>#N/A</c:v>
@@ -1804,13 +1805,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>59.75</c:v>
+                  <c:v>47.75</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>45</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>45</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
@@ -1819,7 +1820,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>45</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>#N/A</c:v>
@@ -1837,16 +1838,16 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>-0.25</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>15</c:v>
+                  <c:v>13.75</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>30</c:v>
+                  <c:v>27.75</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>45</c:v>
+                  <c:v>39.75</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>#N/A</c:v>
@@ -1867,7 +1868,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>59.75</c:v>
+                  <c:v>47.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2036,7 +2037,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -2051,10 +2052,10 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>#N/A</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>#N/A</c:v>
@@ -2075,7 +2076,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>#N/A</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>#N/A</c:v>
@@ -2084,13 +2085,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>#N/A</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>#N/A</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>#N/A</c:v>
@@ -2105,10 +2106,10 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>#N/A</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>#N/A</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>#N/A</c:v>
@@ -2117,7 +2118,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>#N/A</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>#N/A</c:v>
@@ -2141,7 +2142,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>#N/A</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>#N/A</c:v>
@@ -2159,16 +2160,16 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>15</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>15</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>15</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>15</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>#N/A</c:v>
@@ -2358,7 +2359,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
@@ -2373,10 +2374,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>#N/A</c:v>
@@ -2397,7 +2398,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>5</c:v>
@@ -2406,13 +2407,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>#N/A</c:v>
@@ -2427,10 +2428,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>4</c:v>
@@ -2439,7 +2440,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>#N/A</c:v>
@@ -2463,7 +2464,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>#N/A</c:v>
@@ -2680,25 +2681,25 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>#N/A</c:v>
@@ -2710,31 +2711,31 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>#N/A</c:v>
@@ -2746,22 +2747,22 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="27">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="29">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>#N/A</c:v>
@@ -2773,19 +2774,19 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>55</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>50</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>#N/A</c:v>
@@ -2803,16 +2804,16 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>#N/A</c:v>
@@ -2991,10 +2992,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
                 <c:pt idx="0">
-                  <c:v>1.5</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>#N/A</c:v>
@@ -3024,7 +3025,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.5</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>#N/A</c:v>
@@ -3054,13 +3055,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.5</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.5</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>#N/A</c:v>
@@ -3087,7 +3088,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.5</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>#N/A</c:v>
@@ -3120,16 +3121,16 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>#N/A</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>#N/A</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>#N/A</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>#N/A</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>#N/A</c:v>
@@ -3150,7 +3151,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.5</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3710,17 +3711,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:GK130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
@@ -3937,7 +3938,7 @@
     <row r="4" spans="1:193" x14ac:dyDescent="0.2">
       <c r="J4" s="18">
         <f>P62</f>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="M4" s="32"/>
       <c r="N4" s="2" t="s">
@@ -3960,7 +3961,7 @@
     <row r="6" spans="1:193" x14ac:dyDescent="0.2">
       <c r="I6" s="38">
         <f>J4*5</f>
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="J6" s="38"/>
       <c r="K6" s="38"/>
@@ -3980,7 +3981,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:193" ht="35.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:193" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>0</v>
       </c>
@@ -4603,15 +4604,15 @@
       </c>
       <c r="DC9" s="4">
         <f t="shared" ref="DC9:DC26" ca="1" si="14">IF(AC9="","",INDEX($O$9:$O$62,MATCH(AC9,$A$9:$A$62,0)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD9" s="4">
         <f t="shared" ref="DD9:DD26" ca="1" si="15">IF(AD9="","",INDEX($O$9:$O$62,MATCH(AD9,$A$9:$A$62,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="DE9" s="4">
         <f t="shared" ref="DE9:DE26" ca="1" si="16">IF(AE9="","",INDEX($O$9:$O$62,MATCH(AE9,$A$9:$A$62,0)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="DF9" s="4" t="str">
         <f t="shared" ref="DF9:DF26" ca="1" si="17">IF(AF9="","",INDEX($O$9:$O$62,MATCH(AF9,$A$9:$A$62,0)))</f>
@@ -4767,7 +4768,7 @@
       </c>
       <c r="ER9" s="4">
         <f t="shared" ca="1" si="36"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="ES9" s="4" t="str">
         <f t="shared" ca="1" si="36"/>
@@ -4939,7 +4940,7 @@
       </c>
       <c r="GJ9" s="5">
         <f t="shared" ref="GJ9:GJ26" si="55">IF(B9="",NA(),IF(L9=0,$M$62/40,NA()))</f>
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="10" spans="1:193" x14ac:dyDescent="0.2">
@@ -4978,19 +4979,19 @@
       </c>
       <c r="M10" s="8">
         <f t="shared" ref="M10:M62" si="56">MAX(T10:Y10)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N10" s="8">
         <f>M10+L10</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O10" s="8">
         <f t="shared" ref="O10:O62" ca="1" si="57">IF(P10-L10&lt;0,0,P10-L10)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P10" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q10" s="8">
         <f t="shared" ref="Q10:Q62" ca="1" si="58">IF(ROUND(P10-N10,5)&lt;0,0,ROUND(P10-N10,5))</f>
@@ -4998,7 +4999,7 @@
       </c>
       <c r="T10" s="4">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="U10" s="4">
         <f t="shared" si="4"/>
@@ -5382,39 +5383,39 @@
       </c>
       <c r="DM10" s="4">
         <f t="shared" ca="1" si="24"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="DN10" s="4">
         <f t="shared" ca="1" si="25"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="DO10" s="4">
         <f t="shared" ca="1" si="26"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="DP10" s="4">
         <f t="shared" ca="1" si="27"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="DQ10" s="4">
         <f t="shared" ca="1" si="28"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="DR10" s="4">
         <f t="shared" ca="1" si="29"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="DS10" s="4">
         <f t="shared" ca="1" si="30"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="DT10" s="4">
         <f t="shared" ca="1" si="31"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="DU10" s="4">
         <f t="shared" ca="1" si="32"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="DV10" s="4" t="str">
         <f t="shared" ca="1" si="33"/>
@@ -5510,7 +5511,7 @@
       </c>
       <c r="ES10" s="4">
         <f t="shared" ca="1" si="36"/>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="ET10" s="4" t="str">
         <f t="shared" ca="1" si="36"/>
@@ -5546,7 +5547,7 @@
       </c>
       <c r="FB10" s="4">
         <f t="shared" ca="1" si="36"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="FC10" s="4" t="str">
         <f t="shared" ca="1" si="36"/>
@@ -5646,7 +5647,7 @@
       </c>
       <c r="GB10" s="5">
         <f t="shared" si="47"/>
-        <v>14.75</v>
+        <v>13.75</v>
       </c>
       <c r="GC10" s="6" t="e">
         <f t="shared" si="48"/>
@@ -5678,7 +5679,7 @@
       </c>
       <c r="GJ10" s="5">
         <f t="shared" si="55"/>
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="11" spans="1:193" x14ac:dyDescent="0.2">
@@ -5721,15 +5722,15 @@
       </c>
       <c r="O11" s="8">
         <f t="shared" ca="1" si="57"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q11" s="8">
         <f t="shared" ca="1" si="58"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T11" s="4">
         <f t="shared" si="3"/>
@@ -6089,19 +6090,19 @@
       </c>
       <c r="DF11" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="DG11" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="DH11" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="DI11" s="4">
         <f t="shared" ca="1" si="20"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="DJ11" s="4" t="str">
         <f t="shared" ca="1" si="21"/>
@@ -6133,11 +6134,11 @@
       </c>
       <c r="DQ11" s="4">
         <f t="shared" ca="1" si="28"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="DR11" s="4">
         <f t="shared" ca="1" si="29"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="DS11" s="4" t="str">
         <f t="shared" ca="1" si="30"/>
@@ -6149,7 +6150,7 @@
       </c>
       <c r="DU11" s="4">
         <f t="shared" ca="1" si="32"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="DV11" s="4" t="str">
         <f t="shared" ca="1" si="33"/>
@@ -6185,7 +6186,7 @@
       </c>
       <c r="ED11" s="4">
         <f t="shared" ca="1" si="36"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="EE11" s="4" t="str">
         <f t="shared" ca="1" si="36"/>
@@ -6383,33 +6384,33 @@
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
-      <c r="GC11" s="6" t="e">
+      <c r="GC11" s="6">
         <f t="shared" ca="1" si="48"/>
+        <v>4</v>
+      </c>
+      <c r="GD11" s="6">
+        <f t="shared" ca="1" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="GE11" s="6">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="GF11" s="6" t="e">
+        <f t="shared" ca="1" si="51"/>
         <v>#N/A</v>
       </c>
-      <c r="GD11" s="6" t="e">
-        <f t="shared" ca="1" si="49"/>
+      <c r="GG11" s="6" t="e">
+        <f t="shared" ca="1" si="52"/>
         <v>#N/A</v>
       </c>
-      <c r="GE11" s="6" t="e">
-        <f t="shared" ca="1" si="50"/>
+      <c r="GH11" s="6" t="e">
+        <f t="shared" ca="1" si="53"/>
         <v>#N/A</v>
-      </c>
-      <c r="GF11" s="6">
-        <f t="shared" ca="1" si="51"/>
-        <v>4</v>
-      </c>
-      <c r="GG11" s="6">
-        <f t="shared" ca="1" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="GH11" s="6">
-        <f t="shared" ca="1" si="53"/>
-        <v>0</v>
       </c>
       <c r="GI11" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GJ11" s="5" t="e">
         <f t="shared" si="55"/>
@@ -6456,15 +6457,15 @@
       </c>
       <c r="O12" s="8">
         <f t="shared" ca="1" si="57"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P12" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q12" s="8">
         <f t="shared" ca="1" si="58"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T12" s="4">
         <f t="shared" si="3"/>
@@ -6828,7 +6829,7 @@
       </c>
       <c r="DG12" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="DH12" s="4" t="str">
         <f t="shared" ca="1" si="19"/>
@@ -6868,11 +6869,11 @@
       </c>
       <c r="DQ12" s="4">
         <f t="shared" ca="1" si="28"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="DR12" s="4">
         <f t="shared" ca="1" si="29"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="DS12" s="4" t="str">
         <f t="shared" ca="1" si="30"/>
@@ -6884,7 +6885,7 @@
       </c>
       <c r="DU12" s="4">
         <f t="shared" ca="1" si="32"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="DV12" s="4" t="str">
         <f t="shared" ca="1" si="33"/>
@@ -6920,7 +6921,7 @@
       </c>
       <c r="ED12" s="4">
         <f t="shared" ca="1" si="36"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="EE12" s="4" t="str">
         <f t="shared" ca="1" si="36"/>
@@ -7144,7 +7145,7 @@
       </c>
       <c r="GI12" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="GJ12" s="5" t="e">
         <f t="shared" si="55"/>
@@ -7191,15 +7192,15 @@
       </c>
       <c r="O13" s="8">
         <f t="shared" ca="1" si="57"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P13" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q13" s="8">
         <f t="shared" ca="1" si="58"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T13" s="4">
         <f t="shared" si="3"/>
@@ -7559,7 +7560,7 @@
       </c>
       <c r="DF13" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="DG13" s="4" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -7607,19 +7608,19 @@
       </c>
       <c r="DR13" s="4">
         <f t="shared" ca="1" si="29"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="DS13" s="4">
         <f t="shared" ca="1" si="30"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="DT13" s="4">
         <f t="shared" ca="1" si="31"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="DU13" s="4">
         <f t="shared" ca="1" si="32"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="DV13" s="4" t="str">
         <f t="shared" ca="1" si="33"/>
@@ -7635,7 +7636,7 @@
       </c>
       <c r="DY13" s="4">
         <f t="shared" ca="1" si="36"/>
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="DZ13" s="4" t="str">
         <f t="shared" ca="1" si="36"/>
@@ -7879,7 +7880,7 @@
       </c>
       <c r="GI13" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="GJ13" s="5" t="e">
         <f t="shared" si="55"/>
@@ -7928,15 +7929,15 @@
       </c>
       <c r="O14" s="8">
         <f t="shared" ca="1" si="57"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P14" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q14" s="8">
         <f t="shared" ca="1" si="58"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T14" s="4">
         <f t="shared" si="3"/>
@@ -8280,7 +8281,7 @@
       </c>
       <c r="DB14" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="DC14" s="4" t="str">
         <f t="shared" ca="1" si="14"/>
@@ -8340,7 +8341,7 @@
       </c>
       <c r="DQ14" s="4">
         <f t="shared" ca="1" si="28"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="DR14" s="4" t="str">
         <f t="shared" ca="1" si="29"/>
@@ -8616,7 +8617,7 @@
       </c>
       <c r="GI14" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="GJ14" s="5" t="e">
         <f t="shared" si="55"/>
@@ -8665,15 +8666,15 @@
       </c>
       <c r="O15" s="8">
         <f t="shared" ca="1" si="57"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P15" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q15" s="8">
         <f t="shared" ca="1" si="58"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T15" s="4">
         <f t="shared" si="3"/>
@@ -9017,7 +9018,7 @@
       </c>
       <c r="DB15" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="DC15" s="4" t="str">
         <f t="shared" ca="1" si="14"/>
@@ -9081,11 +9082,11 @@
       </c>
       <c r="DR15" s="4">
         <f t="shared" ca="1" si="29"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="DS15" s="4">
         <f t="shared" ca="1" si="30"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="DT15" s="4" t="str">
         <f t="shared" ca="1" si="31"/>
@@ -9353,7 +9354,7 @@
       </c>
       <c r="GI15" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="GJ15" s="5" t="e">
         <f t="shared" si="55"/>
@@ -9402,15 +9403,15 @@
       </c>
       <c r="O16" s="8">
         <f t="shared" ca="1" si="57"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P16" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q16" s="8">
         <f t="shared" ca="1" si="58"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16" s="4">
         <f t="shared" si="3"/>
@@ -9754,7 +9755,7 @@
       </c>
       <c r="DB16" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="DC16" s="4" t="str">
         <f t="shared" ca="1" si="14"/>
@@ -9810,7 +9811,7 @@
       </c>
       <c r="DP16" s="4">
         <f t="shared" ca="1" si="27"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="DQ16" s="4" t="str">
         <f t="shared" ca="1" si="28"/>
@@ -9822,7 +9823,7 @@
       </c>
       <c r="DS16" s="4">
         <f t="shared" ca="1" si="30"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="DT16" s="4" t="str">
         <f t="shared" ca="1" si="31"/>
@@ -10064,33 +10065,33 @@
         <f t="shared" si="47"/>
         <v>10</v>
       </c>
-      <c r="GC16" s="6" t="e">
+      <c r="GC16" s="6">
         <f t="shared" ca="1" si="48"/>
+        <v>4</v>
+      </c>
+      <c r="GD16" s="6">
+        <f t="shared" ca="1" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="GE16" s="6">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="GF16" s="6" t="e">
+        <f t="shared" ca="1" si="51"/>
         <v>#N/A</v>
       </c>
-      <c r="GD16" s="6" t="e">
-        <f t="shared" ca="1" si="49"/>
+      <c r="GG16" s="6" t="e">
+        <f t="shared" ca="1" si="52"/>
         <v>#N/A</v>
       </c>
-      <c r="GE16" s="6" t="e">
-        <f t="shared" ca="1" si="50"/>
+      <c r="GH16" s="6" t="e">
+        <f t="shared" ca="1" si="53"/>
         <v>#N/A</v>
-      </c>
-      <c r="GF16" s="6">
-        <f t="shared" ca="1" si="51"/>
-        <v>4</v>
-      </c>
-      <c r="GG16" s="6">
-        <f t="shared" ca="1" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="GH16" s="6">
-        <f t="shared" ca="1" si="53"/>
-        <v>0</v>
       </c>
       <c r="GI16" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GJ16" s="5" t="e">
         <f t="shared" si="55"/>
@@ -10137,15 +10138,15 @@
       </c>
       <c r="O17" s="8">
         <f t="shared" ref="O17:O25" ca="1" si="67">IF(P17-L17&lt;0,0,P17-L17)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P17" s="8">
         <f t="shared" ref="P17:P25" ca="1" si="68">MIN(DA17:FZ17)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q17" s="8">
         <f t="shared" ref="Q17:Q25" ca="1" si="69">IF(ROUND(P17-N17,5)&lt;0,0,ROUND(P17-N17,5))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17" s="4">
         <f t="shared" ref="T17:T25" si="70">IF(C17="",0,INDEX($N$9:$N$62,MATCH(C17,$A$9:$A$62,0)))</f>
@@ -10513,7 +10514,7 @@
       </c>
       <c r="DH17" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="DI17" s="4" t="str">
         <f t="shared" ca="1" si="20"/>
@@ -10545,7 +10546,7 @@
       </c>
       <c r="DP17" s="4">
         <f t="shared" ca="1" si="27"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="DQ17" s="4" t="str">
         <f t="shared" ca="1" si="28"/>
@@ -10799,33 +10800,33 @@
         <f t="shared" si="47"/>
         <v>4</v>
       </c>
-      <c r="GC17" s="6" t="e">
+      <c r="GC17" s="6">
         <f t="shared" ca="1" si="48"/>
+        <v>6</v>
+      </c>
+      <c r="GD17" s="6">
+        <f t="shared" ca="1" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="GE17" s="6">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="GF17" s="6" t="e">
+        <f t="shared" ca="1" si="51"/>
         <v>#N/A</v>
       </c>
-      <c r="GD17" s="6" t="e">
-        <f t="shared" ca="1" si="49"/>
+      <c r="GG17" s="6" t="e">
+        <f t="shared" ca="1" si="52"/>
         <v>#N/A</v>
       </c>
-      <c r="GE17" s="6" t="e">
-        <f t="shared" ca="1" si="50"/>
+      <c r="GH17" s="6" t="e">
+        <f t="shared" ca="1" si="53"/>
         <v>#N/A</v>
-      </c>
-      <c r="GF17" s="6">
-        <f t="shared" ca="1" si="51"/>
-        <v>6</v>
-      </c>
-      <c r="GG17" s="6">
-        <f t="shared" ca="1" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="GH17" s="6">
-        <f t="shared" ca="1" si="53"/>
-        <v>0</v>
       </c>
       <c r="GI17" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GJ17" s="5" t="e">
         <f t="shared" si="55"/>
@@ -12328,19 +12329,19 @@
       </c>
       <c r="M20" s="8">
         <f t="shared" si="65"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N20" s="8">
         <f t="shared" si="66"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O20" s="8">
         <f t="shared" ca="1" si="67"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P20" s="8">
         <f t="shared" ca="1" si="68"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q20" s="8">
         <f t="shared" ca="1" si="69"/>
@@ -12348,23 +12349,23 @@
       </c>
       <c r="T20" s="4">
         <f t="shared" si="70"/>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="U20" s="4">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V20" s="4">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="W20" s="4">
         <f t="shared" si="6"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X20" s="4">
         <f t="shared" si="7"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y20" s="4">
         <f t="shared" si="8"/>
@@ -12780,27 +12781,27 @@
       </c>
       <c r="DY20" s="4">
         <f t="shared" ca="1" si="63"/>
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="DZ20" s="4">
         <f t="shared" ca="1" si="63"/>
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="EA20" s="4">
         <f t="shared" ca="1" si="63"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="EB20" s="4">
         <f t="shared" ca="1" si="63"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="EC20" s="4">
         <f t="shared" ca="1" si="63"/>
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="ED20" s="4">
         <f t="shared" ca="1" si="63"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="EE20" s="4" t="str">
         <f t="shared" ca="1" si="63"/>
@@ -12864,7 +12865,7 @@
       </c>
       <c r="ET20" s="4">
         <f t="shared" ca="1" si="62"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="EU20" s="4" t="str">
         <f t="shared" ca="1" si="62"/>
@@ -12896,7 +12897,7 @@
       </c>
       <c r="FB20" s="4">
         <f t="shared" ca="1" si="62"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="FC20" s="4" t="str">
         <f t="shared" ca="1" si="62"/>
@@ -12996,7 +12997,7 @@
       </c>
       <c r="GB20" s="5">
         <f t="shared" si="47"/>
-        <v>29.75</v>
+        <v>27.75</v>
       </c>
       <c r="GC20" s="6" t="e">
         <f t="shared" si="48"/>
@@ -13028,7 +13029,7 @@
       </c>
       <c r="GJ20" s="5">
         <f t="shared" si="55"/>
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="21" spans="1:192" x14ac:dyDescent="0.2">
@@ -13065,31 +13066,31 @@
       </c>
       <c r="M21" s="8">
         <f t="shared" si="65"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N21" s="8">
         <f t="shared" si="66"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O21" s="8">
         <f t="shared" ca="1" si="67"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P21" s="8">
         <f t="shared" ca="1" si="68"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Q21" s="8">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T21" s="4">
         <f t="shared" si="70"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U21" s="4">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V21" s="4">
         <f t="shared" si="5"/>
@@ -13477,7 +13478,7 @@
       </c>
       <c r="DO21" s="4">
         <f t="shared" ca="1" si="26"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="DP21" s="4" t="str">
         <f t="shared" ca="1" si="27"/>
@@ -13505,7 +13506,7 @@
       </c>
       <c r="DV21" s="4">
         <f t="shared" ca="1" si="33"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="DW21" s="4" t="str">
         <f t="shared" ca="1" si="34"/>
@@ -13733,7 +13734,7 @@
       </c>
       <c r="GB21" s="5">
         <f t="shared" si="47"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="GC21" s="6" t="e">
         <f t="shared" ca="1" si="48"/>
@@ -13761,7 +13762,7 @@
       </c>
       <c r="GI21" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="GJ21" s="5" t="e">
         <f t="shared" si="55"/>
@@ -13802,31 +13803,31 @@
       </c>
       <c r="M22" s="8">
         <f t="shared" si="65"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N22" s="8">
         <f t="shared" si="66"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O22" s="8">
         <f t="shared" ca="1" si="67"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" ca="1" si="68"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q22" s="8">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T22" s="4">
         <f t="shared" si="70"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U22" s="4">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V22" s="4">
         <f t="shared" si="5"/>
@@ -14234,7 +14235,7 @@
       </c>
       <c r="DT22" s="4">
         <f t="shared" ca="1" si="31"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="DU22" s="4" t="str">
         <f t="shared" ca="1" si="32"/>
@@ -14242,7 +14243,7 @@
       </c>
       <c r="DV22" s="4">
         <f t="shared" ca="1" si="33"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="DW22" s="4" t="str">
         <f t="shared" ca="1" si="34"/>
@@ -14470,7 +14471,7 @@
       </c>
       <c r="GB22" s="5">
         <f t="shared" si="47"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="GC22" s="6" t="e">
         <f t="shared" ca="1" si="48"/>
@@ -14498,7 +14499,7 @@
       </c>
       <c r="GI22" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="GJ22" s="5" t="e">
         <f t="shared" si="55"/>
@@ -14539,31 +14540,31 @@
       </c>
       <c r="M23" s="8">
         <f t="shared" si="65"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N23" s="8">
         <f t="shared" si="66"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O23" s="8">
         <f t="shared" ca="1" si="67"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P23" s="8">
         <f t="shared" ca="1" si="68"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q23" s="8">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T23" s="4">
         <f t="shared" si="70"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U23" s="4">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V23" s="4">
         <f t="shared" si="5"/>
@@ -14979,7 +14980,7 @@
       </c>
       <c r="DV23" s="4">
         <f t="shared" ca="1" si="33"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="DW23" s="4" t="str">
         <f t="shared" ca="1" si="34"/>
@@ -14991,7 +14992,7 @@
       </c>
       <c r="DY23" s="4">
         <f t="shared" ca="1" si="63"/>
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="DZ23" s="4" t="str">
         <f t="shared" ca="1" si="63"/>
@@ -15207,7 +15208,7 @@
       </c>
       <c r="GB23" s="5">
         <f t="shared" si="47"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="GC23" s="6" t="e">
         <f t="shared" ca="1" si="48"/>
@@ -15235,7 +15236,7 @@
       </c>
       <c r="GI23" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="GJ23" s="5" t="e">
         <f t="shared" si="55"/>
@@ -15278,23 +15279,23 @@
       </c>
       <c r="M24" s="8">
         <f t="shared" si="65"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N24" s="8">
         <f t="shared" si="66"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O24" s="8">
         <f t="shared" ca="1" si="67"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P24" s="8">
         <f t="shared" ca="1" si="68"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q24" s="8">
         <f t="shared" ca="1" si="69"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T24" s="4">
         <f t="shared" si="70"/>
@@ -15302,7 +15303,7 @@
       </c>
       <c r="U24" s="4">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V24" s="4">
         <f t="shared" si="5"/>
@@ -15706,7 +15707,7 @@
       </c>
       <c r="DS24" s="4">
         <f t="shared" ca="1" si="30"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="DT24" s="4" t="str">
         <f t="shared" ca="1" si="31"/>
@@ -15718,7 +15719,7 @@
       </c>
       <c r="DV24" s="4">
         <f t="shared" ca="1" si="33"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="DW24" s="4" t="str">
         <f t="shared" ca="1" si="34"/>
@@ -15946,35 +15947,35 @@
       </c>
       <c r="GB24" s="5">
         <f t="shared" si="47"/>
-        <v>15</v>
-      </c>
-      <c r="GC24" s="6" t="e">
+        <v>14</v>
+      </c>
+      <c r="GC24" s="6">
         <f t="shared" ca="1" si="48"/>
+        <v>5</v>
+      </c>
+      <c r="GD24" s="6">
+        <f t="shared" ca="1" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="GE24" s="6">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="GF24" s="6" t="e">
+        <f t="shared" ca="1" si="51"/>
         <v>#N/A</v>
       </c>
-      <c r="GD24" s="6" t="e">
-        <f t="shared" ca="1" si="49"/>
+      <c r="GG24" s="6" t="e">
+        <f t="shared" ca="1" si="52"/>
         <v>#N/A</v>
       </c>
-      <c r="GE24" s="6" t="e">
-        <f t="shared" ca="1" si="50"/>
+      <c r="GH24" s="6" t="e">
+        <f t="shared" ca="1" si="53"/>
         <v>#N/A</v>
-      </c>
-      <c r="GF24" s="6">
-        <f t="shared" ca="1" si="51"/>
-        <v>5</v>
-      </c>
-      <c r="GG24" s="6">
-        <f t="shared" ca="1" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="GH24" s="6">
-        <f t="shared" ca="1" si="53"/>
-        <v>0</v>
       </c>
       <c r="GI24" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GJ24" s="5" t="e">
         <f t="shared" si="55"/>
@@ -16019,23 +16020,23 @@
       </c>
       <c r="M25" s="8">
         <f t="shared" si="65"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N25" s="8">
         <f t="shared" si="66"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O25" s="8">
         <f t="shared" ca="1" si="67"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P25" s="8">
         <f t="shared" ca="1" si="68"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q25" s="8">
         <f t="shared" ca="1" si="69"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T25" s="4">
         <f t="shared" si="70"/>
@@ -16043,7 +16044,7 @@
       </c>
       <c r="U25" s="4">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V25" s="4">
         <f t="shared" si="5"/>
@@ -16423,7 +16424,7 @@
       </c>
       <c r="DM25" s="4">
         <f t="shared" ca="1" si="24"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="DN25" s="4" t="str">
         <f t="shared" ca="1" si="25"/>
@@ -16687,7 +16688,7 @@
       </c>
       <c r="GB25" s="5">
         <f t="shared" si="47"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="GC25" s="6" t="e">
         <f t="shared" ca="1" si="48"/>
@@ -16715,7 +16716,7 @@
       </c>
       <c r="GI25" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="GJ25" s="5" t="e">
         <f t="shared" si="55"/>
@@ -16762,23 +16763,23 @@
       </c>
       <c r="M26" s="8">
         <f t="shared" ref="M26" si="80">MAX(T26:Y26)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N26" s="8">
         <f t="shared" ref="N26" si="81">M26+L26</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O26" s="8">
         <f t="shared" ref="O26" ca="1" si="82">IF(P26-L26&lt;0,0,P26-L26)</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P26" s="8">
         <f ca="1">MIN(DA26:FZ26)</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q26" s="8">
         <f t="shared" ref="Q26" ca="1" si="83">IF(ROUND(P26-N26,5)&lt;0,0,ROUND(P26-N26,5))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T26" s="4">
         <f t="shared" ref="T26" si="84">IF(C26="",0,INDEX($N$9:$N$62,MATCH(C26,$A$9:$A$62,0)))</f>
@@ -16786,7 +16787,7 @@
       </c>
       <c r="U26" s="4">
         <f t="shared" ref="U26" si="85">IF(D26="",0,INDEX($N$9:$N$62,MATCH(D26,$A$9:$A$62,0)))</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V26" s="4">
         <f t="shared" ref="V26" si="86">IF(E26="",0,INDEX($N$9:$N$62,MATCH(E26,$A$9:$A$62,0)))</f>
@@ -17170,7 +17171,7 @@
       </c>
       <c r="DN26" s="4">
         <f t="shared" ca="1" si="25"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="DO26" s="4" t="str">
         <f t="shared" ca="1" si="26"/>
@@ -17430,7 +17431,7 @@
       </c>
       <c r="GB26" s="5">
         <f t="shared" si="47"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="GC26" s="6" t="e">
         <f t="shared" ca="1" si="48"/>
@@ -17458,7 +17459,7 @@
       </c>
       <c r="GI26" s="5">
         <f t="shared" ca="1" si="54"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="GJ26" s="5" t="e">
         <f t="shared" si="55"/>
@@ -17507,31 +17508,31 @@
       </c>
       <c r="M27" s="8">
         <f t="shared" ref="M27:M61" si="89">MAX(T27:Y27)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N27" s="8">
         <f t="shared" ref="N27:N61" si="90">M27+L27</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O27" s="8">
         <f t="shared" ref="O27:O61" ca="1" si="91">IF(P27-L27&lt;0,0,P27-L27)</f>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P27" s="8">
         <f t="shared" ref="P27:P61" ca="1" si="92">MIN(DA27:FZ27)</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Q27" s="8">
         <f t="shared" ref="Q27:Q61" ca="1" si="93">IF(ROUND(P27-N27,5)&lt;0,0,ROUND(P27-N27,5))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T27" s="4">
         <f t="shared" ref="T27:T61" si="94">IF(C27="",0,INDEX($N$9:$N$62,MATCH(C27,$A$9:$A$62,0)))</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U27" s="4">
         <f t="shared" ref="U27:U61" si="95">IF(D27="",0,INDEX($N$9:$N$62,MATCH(D27,$A$9:$A$62,0)))</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V27" s="4">
         <f t="shared" ref="V27:V61" si="96">IF(E27="",0,INDEX($N$9:$N$62,MATCH(E27,$A$9:$A$62,0)))</f>
@@ -17547,7 +17548,7 @@
       </c>
       <c r="Y27" s="4">
         <f t="shared" ref="Y27:Y61" si="99">IF(H27="",0,INDEX($N$9:$N$62,MATCH(H27,$A$9:$A$62,0)))</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AA27" s="4" t="str">
         <f t="shared" ca="1" si="72"/>
@@ -17907,7 +17908,7 @@
       </c>
       <c r="DL27" s="4">
         <f t="shared" ref="DL27:DL61" ca="1" si="111">IF(AL27="","",INDEX($O$9:$O$62,MATCH(AL27,$A$9:$A$62,0)))</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="DM27" s="4" t="str">
         <f t="shared" ref="DM27:DM61" ca="1" si="112">IF(AM27="","",INDEX($O$9:$O$62,MATCH(AM27,$A$9:$A$62,0)))</f>
@@ -17943,7 +17944,7 @@
       </c>
       <c r="DU27" s="4">
         <f t="shared" ref="DU27:DU61" ca="1" si="120">IF(AU27="","",INDEX($O$9:$O$62,MATCH(AU27,$A$9:$A$62,0)))</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="DV27" s="4" t="str">
         <f t="shared" ref="DV27:DV61" ca="1" si="121">IF(AV27="","",INDEX($O$9:$O$62,MATCH(AV27,$A$9:$A$62,0)))</f>
@@ -18175,35 +18176,35 @@
       </c>
       <c r="GB27" s="5">
         <f t="shared" ref="GB27:GB61" si="124">IF(B27="",NA(),IF(L27=0,M27-0.25,M27))</f>
-        <v>20</v>
-      </c>
-      <c r="GC27" s="6" t="e">
+        <v>19</v>
+      </c>
+      <c r="GC27" s="6">
         <f t="shared" ref="GC27:GC61" ca="1" si="125">IF(B27="",NA(),IF(L27=0,NA(),IF(Q27&lt;=0.01,L27,NA())))</f>
+        <v>5</v>
+      </c>
+      <c r="GD27" s="6">
+        <f t="shared" ref="GD27:GD61" ca="1" si="126">IF(B27="",NA(),IF(ISERROR(GC27),NA(),K27-L27))</f>
+        <v>0</v>
+      </c>
+      <c r="GE27" s="6">
+        <f t="shared" ref="GE27:GE61" ca="1" si="127">IF(B27="",NA(),IF(ISERROR(GC27),NA(),L27-I27))</f>
+        <v>0</v>
+      </c>
+      <c r="GF27" s="6" t="e">
+        <f t="shared" ref="GF27:GF61" ca="1" si="128">IF(B27="",NA(),IF(L27=0,NA(),IF(Q27&gt;0,L27,NA())))</f>
         <v>#N/A</v>
       </c>
-      <c r="GD27" s="6" t="e">
-        <f t="shared" ref="GD27:GD61" ca="1" si="126">IF(B27="",NA(),IF(ISERROR(GC27),NA(),K27-L27))</f>
+      <c r="GG27" s="6" t="e">
+        <f t="shared" ref="GG27:GG61" ca="1" si="129">IF(B27="",NA(),IF(ISERROR(GF27),NA(),K27-L27))</f>
         <v>#N/A</v>
       </c>
-      <c r="GE27" s="6" t="e">
-        <f t="shared" ref="GE27:GE61" ca="1" si="127">IF(B27="",NA(),IF(ISERROR(GC27),NA(),L27-I27))</f>
+      <c r="GH27" s="6" t="e">
+        <f t="shared" ref="GH27:GH61" ca="1" si="130">IF(B27="",NA(),IF(ISERROR(GF27),NA(),L27-I27))</f>
         <v>#N/A</v>
-      </c>
-      <c r="GF27" s="6">
-        <f t="shared" ref="GF27:GF61" ca="1" si="128">IF(B27="",NA(),IF(L27=0,NA(),IF(Q27&gt;0,L27,NA())))</f>
-        <v>5</v>
-      </c>
-      <c r="GG27" s="6">
-        <f t="shared" ref="GG27:GG61" ca="1" si="129">IF(B27="",NA(),IF(ISERROR(GF27),NA(),K27-L27))</f>
-        <v>0</v>
-      </c>
-      <c r="GH27" s="6">
-        <f t="shared" ref="GH27:GH61" ca="1" si="130">IF(B27="",NA(),IF(ISERROR(GF27),NA(),L27-I27))</f>
-        <v>0</v>
       </c>
       <c r="GI27" s="5">
         <f t="shared" ref="GI27:GI61" ca="1" si="131">IF(B27="",NA(),IF(L27=0,NA(),Q27))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GJ27" s="5" t="e">
         <f t="shared" ref="GJ27:GJ61" si="132">IF(B27="",NA(),IF(L27=0,$M$62/40,NA()))</f>
@@ -18246,31 +18247,31 @@
       </c>
       <c r="M28" s="8">
         <f t="shared" si="89"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N28" s="8">
         <f t="shared" si="90"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O28" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="P28" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q28" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T28" s="4">
         <f t="shared" si="94"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U28" s="4">
         <f t="shared" si="95"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V28" s="4">
         <f t="shared" si="96"/>
@@ -18646,7 +18647,7 @@
       </c>
       <c r="DL28" s="4">
         <f t="shared" ca="1" si="111"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="DM28" s="4" t="str">
         <f t="shared" ca="1" si="112"/>
@@ -18702,7 +18703,7 @@
       </c>
       <c r="DZ28" s="4">
         <f t="shared" ca="1" si="63"/>
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="EA28" s="4" t="str">
         <f t="shared" ca="1" si="63"/>
@@ -18914,7 +18915,7 @@
       </c>
       <c r="GB28" s="5">
         <f t="shared" si="124"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="GC28" s="6" t="e">
         <f t="shared" ca="1" si="125"/>
@@ -18942,7 +18943,7 @@
       </c>
       <c r="GI28" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="GJ28" s="5" t="e">
         <f t="shared" si="132"/>
@@ -18989,31 +18990,31 @@
       </c>
       <c r="M29" s="8">
         <f t="shared" si="89"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N29" s="8">
         <f t="shared" si="90"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O29" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q29" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T29" s="4">
         <f t="shared" si="94"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U29" s="4">
         <f t="shared" si="95"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V29" s="4">
         <f t="shared" si="96"/>
@@ -19389,7 +19390,7 @@
       </c>
       <c r="DL29" s="4">
         <f t="shared" ca="1" si="111"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="DM29" s="4" t="str">
         <f t="shared" ca="1" si="112"/>
@@ -19449,7 +19450,7 @@
       </c>
       <c r="EA29" s="4">
         <f t="shared" ca="1" si="63"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="EB29" s="4" t="str">
         <f t="shared" ca="1" si="63"/>
@@ -19657,35 +19658,35 @@
       </c>
       <c r="GB29" s="5">
         <f t="shared" si="124"/>
-        <v>25</v>
-      </c>
-      <c r="GC29" s="6" t="e">
+        <v>24</v>
+      </c>
+      <c r="GC29" s="6">
         <f t="shared" ca="1" si="125"/>
+        <v>4</v>
+      </c>
+      <c r="GD29" s="6">
+        <f t="shared" ca="1" si="126"/>
+        <v>0</v>
+      </c>
+      <c r="GE29" s="6">
+        <f t="shared" ca="1" si="127"/>
+        <v>0</v>
+      </c>
+      <c r="GF29" s="6" t="e">
+        <f t="shared" ca="1" si="128"/>
         <v>#N/A</v>
       </c>
-      <c r="GD29" s="6" t="e">
-        <f t="shared" ca="1" si="126"/>
+      <c r="GG29" s="6" t="e">
+        <f t="shared" ca="1" si="129"/>
         <v>#N/A</v>
       </c>
-      <c r="GE29" s="6" t="e">
-        <f t="shared" ca="1" si="127"/>
+      <c r="GH29" s="6" t="e">
+        <f t="shared" ca="1" si="130"/>
         <v>#N/A</v>
-      </c>
-      <c r="GF29" s="6">
-        <f t="shared" ca="1" si="128"/>
-        <v>4</v>
-      </c>
-      <c r="GG29" s="6">
-        <f t="shared" ca="1" si="129"/>
-        <v>0</v>
-      </c>
-      <c r="GH29" s="6">
-        <f t="shared" ca="1" si="130"/>
-        <v>0</v>
       </c>
       <c r="GI29" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GJ29" s="5" t="e">
         <f t="shared" si="132"/>
@@ -19730,39 +19731,39 @@
       </c>
       <c r="M30" s="8">
         <f t="shared" si="89"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N30" s="8">
         <f t="shared" si="90"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O30" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P30" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q30" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T30" s="4">
         <f t="shared" si="94"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U30" s="4">
         <f t="shared" si="95"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="V30" s="4">
         <f t="shared" si="96"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W30" s="4">
         <f t="shared" si="97"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="X30" s="4">
         <f t="shared" si="98"/>
@@ -20130,7 +20131,7 @@
       </c>
       <c r="DL30" s="4">
         <f t="shared" ca="1" si="111"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="DM30" s="4" t="str">
         <f t="shared" ca="1" si="112"/>
@@ -20398,7 +20399,7 @@
       </c>
       <c r="GB30" s="5">
         <f t="shared" si="124"/>
-        <v>27.75</v>
+        <v>26.75</v>
       </c>
       <c r="GC30" s="6" t="e">
         <f t="shared" si="125"/>
@@ -20430,7 +20431,7 @@
       </c>
       <c r="GJ30" s="5">
         <f t="shared" si="132"/>
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="31" spans="1:192" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -21202,19 +21203,19 @@
       </c>
       <c r="M32" s="8">
         <f t="shared" si="89"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="N32" s="8">
         <f t="shared" si="90"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="O32" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="P32" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="Q32" s="8">
         <f t="shared" ca="1" si="93"/>
@@ -21222,27 +21223,27 @@
       </c>
       <c r="T32" s="4">
         <f t="shared" si="94"/>
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="U32" s="4">
         <f t="shared" si="95"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="V32" s="4">
         <f t="shared" si="96"/>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="W32" s="4">
         <f t="shared" si="97"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="X32" s="4">
         <f t="shared" si="98"/>
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Y32" s="4">
         <f t="shared" si="99"/>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AA32" s="4" t="str">
         <f t="shared" ca="1" si="72"/>
@@ -21690,11 +21691,11 @@
       </c>
       <c r="EH32" s="4">
         <f t="shared" ca="1" si="144"/>
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="EI32" s="4">
         <f t="shared" ca="1" si="76"/>
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="EJ32" s="4" t="str">
         <f t="shared" ca="1" si="76"/>
@@ -21706,7 +21707,7 @@
       </c>
       <c r="EL32" s="4">
         <f t="shared" ca="1" si="76"/>
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="EM32" s="4" t="str">
         <f t="shared" ca="1" si="76"/>
@@ -21742,7 +21743,7 @@
       </c>
       <c r="EU32" s="4">
         <f t="shared" ca="1" si="76"/>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="EV32" s="4" t="str">
         <f t="shared" ca="1" si="76"/>
@@ -21770,7 +21771,7 @@
       </c>
       <c r="FB32" s="4">
         <f t="shared" ca="1" si="76"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="FC32" s="4" t="str">
         <f t="shared" ca="1" si="76"/>
@@ -21870,7 +21871,7 @@
       </c>
       <c r="GB32" s="5">
         <f t="shared" si="124"/>
-        <v>44.75</v>
+        <v>39.75</v>
       </c>
       <c r="GC32" s="6" t="e">
         <f t="shared" si="125"/>
@@ -21902,7 +21903,7 @@
       </c>
       <c r="GJ32" s="5">
         <f t="shared" si="132"/>
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="33" spans="1:192" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -21941,31 +21942,31 @@
       </c>
       <c r="M33" s="8">
         <f t="shared" si="89"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N33" s="8">
         <f t="shared" si="90"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O33" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P33" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Q33" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="T33" s="4">
         <f t="shared" si="94"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U33" s="4">
         <f t="shared" si="95"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V33" s="4">
         <f t="shared" si="96"/>
@@ -22389,7 +22390,7 @@
       </c>
       <c r="DX33" s="4">
         <f t="shared" ca="1" si="123"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="DY33" s="4" t="str">
         <f t="shared" ca="1" si="135"/>
@@ -22405,7 +22406,7 @@
       </c>
       <c r="EB33" s="4">
         <f t="shared" ca="1" si="138"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="EC33" s="4" t="str">
         <f t="shared" ca="1" si="139"/>
@@ -22609,7 +22610,7 @@
       </c>
       <c r="GB33" s="5">
         <f t="shared" si="124"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="GC33" s="6" t="e">
         <f t="shared" ca="1" si="125"/>
@@ -22637,7 +22638,7 @@
       </c>
       <c r="GI33" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="GJ33" s="5" t="e">
         <f t="shared" si="132"/>
@@ -22678,31 +22679,31 @@
       </c>
       <c r="M34" s="8">
         <f t="shared" si="89"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N34" s="8">
         <f t="shared" si="90"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O34" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="P34" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="Q34" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T34" s="4">
         <f t="shared" si="94"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U34" s="4">
         <f t="shared" si="95"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V34" s="4">
         <f t="shared" si="96"/>
@@ -23138,7 +23139,7 @@
       </c>
       <c r="EA34" s="4">
         <f t="shared" ca="1" si="137"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="EB34" s="4" t="str">
         <f t="shared" ca="1" si="138"/>
@@ -23150,7 +23151,7 @@
       </c>
       <c r="ED34" s="4">
         <f t="shared" ca="1" si="140"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="EE34" s="4" t="str">
         <f t="shared" ca="1" si="141"/>
@@ -23346,35 +23347,35 @@
       </c>
       <c r="GB34" s="5">
         <f t="shared" si="124"/>
-        <v>30</v>
-      </c>
-      <c r="GC34" s="6" t="e">
+        <v>28</v>
+      </c>
+      <c r="GC34" s="6">
         <f t="shared" ca="1" si="125"/>
+        <v>7</v>
+      </c>
+      <c r="GD34" s="6">
+        <f t="shared" ca="1" si="126"/>
+        <v>0</v>
+      </c>
+      <c r="GE34" s="6">
+        <f t="shared" ca="1" si="127"/>
+        <v>0</v>
+      </c>
+      <c r="GF34" s="6" t="e">
+        <f t="shared" ca="1" si="128"/>
         <v>#N/A</v>
       </c>
-      <c r="GD34" s="6" t="e">
-        <f t="shared" ca="1" si="126"/>
+      <c r="GG34" s="6" t="e">
+        <f t="shared" ca="1" si="129"/>
         <v>#N/A</v>
       </c>
-      <c r="GE34" s="6" t="e">
-        <f t="shared" ca="1" si="127"/>
+      <c r="GH34" s="6" t="e">
+        <f t="shared" ca="1" si="130"/>
         <v>#N/A</v>
-      </c>
-      <c r="GF34" s="6">
-        <f t="shared" ca="1" si="128"/>
-        <v>7</v>
-      </c>
-      <c r="GG34" s="6">
-        <f t="shared" ca="1" si="129"/>
-        <v>0</v>
-      </c>
-      <c r="GH34" s="6">
-        <f t="shared" ca="1" si="130"/>
-        <v>0</v>
       </c>
       <c r="GI34" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="GJ34" s="5" t="e">
         <f t="shared" si="132"/>
@@ -23417,35 +23418,35 @@
       </c>
       <c r="M35" s="8">
         <f t="shared" si="89"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N35" s="8">
         <f t="shared" si="90"/>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O35" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="P35" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="Q35" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T35" s="4">
         <f t="shared" si="94"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U35" s="4">
         <f t="shared" si="95"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V35" s="4">
         <f t="shared" si="96"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="W35" s="4">
         <f t="shared" si="97"/>
@@ -23865,7 +23866,7 @@
       </c>
       <c r="DX35" s="4">
         <f t="shared" ca="1" si="123"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="DY35" s="4" t="str">
         <f t="shared" ca="1" si="135"/>
@@ -24085,35 +24086,35 @@
       </c>
       <c r="GB35" s="5">
         <f t="shared" si="124"/>
-        <v>37</v>
-      </c>
-      <c r="GC35" s="6" t="e">
+        <v>35</v>
+      </c>
+      <c r="GC35" s="6">
         <f t="shared" ca="1" si="125"/>
+        <v>5</v>
+      </c>
+      <c r="GD35" s="6">
+        <f t="shared" ca="1" si="126"/>
+        <v>0</v>
+      </c>
+      <c r="GE35" s="6">
+        <f t="shared" ca="1" si="127"/>
+        <v>0</v>
+      </c>
+      <c r="GF35" s="6" t="e">
+        <f t="shared" ca="1" si="128"/>
         <v>#N/A</v>
       </c>
-      <c r="GD35" s="6" t="e">
-        <f t="shared" ca="1" si="126"/>
+      <c r="GG35" s="6" t="e">
+        <f t="shared" ca="1" si="129"/>
         <v>#N/A</v>
       </c>
-      <c r="GE35" s="6" t="e">
-        <f t="shared" ca="1" si="127"/>
+      <c r="GH35" s="6" t="e">
+        <f t="shared" ca="1" si="130"/>
         <v>#N/A</v>
-      </c>
-      <c r="GF35" s="6">
-        <f t="shared" ca="1" si="128"/>
-        <v>5</v>
-      </c>
-      <c r="GG35" s="6">
-        <f t="shared" ca="1" si="129"/>
-        <v>0</v>
-      </c>
-      <c r="GH35" s="6">
-        <f t="shared" ca="1" si="130"/>
-        <v>0</v>
       </c>
       <c r="GI35" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="GJ35" s="5" t="e">
         <f t="shared" si="132"/>
@@ -24156,35 +24157,35 @@
       </c>
       <c r="M36" s="8">
         <f t="shared" si="89"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N36" s="8">
         <f t="shared" si="90"/>
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O36" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="P36" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="Q36" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T36" s="4">
         <f t="shared" si="94"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U36" s="4">
         <f t="shared" si="95"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V36" s="4">
         <f t="shared" si="96"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="W36" s="4">
         <f t="shared" si="97"/>
@@ -24604,7 +24605,7 @@
       </c>
       <c r="DX36" s="4">
         <f t="shared" ca="1" si="123"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="DY36" s="4" t="str">
         <f t="shared" ca="1" si="135"/>
@@ -24648,7 +24649,7 @@
       </c>
       <c r="EI36" s="4">
         <f t="shared" ca="1" si="164"/>
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="EJ36" s="4" t="str">
         <f t="shared" ca="1" si="165"/>
@@ -24824,7 +24825,7 @@
       </c>
       <c r="GB36" s="5">
         <f t="shared" si="124"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="GC36" s="6" t="e">
         <f t="shared" ca="1" si="125"/>
@@ -24852,7 +24853,7 @@
       </c>
       <c r="GI36" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="GJ36" s="5" t="e">
         <f t="shared" si="132"/>
@@ -24891,23 +24892,23 @@
       </c>
       <c r="M37" s="8">
         <f t="shared" si="89"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N37" s="8">
         <f t="shared" si="90"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O37" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="P37" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Q37" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T37" s="4">
         <f t="shared" si="94"/>
@@ -24915,7 +24916,7 @@
       </c>
       <c r="U37" s="4">
         <f t="shared" si="95"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V37" s="4">
         <f t="shared" si="96"/>
@@ -25339,7 +25340,7 @@
       </c>
       <c r="DX37" s="4">
         <f t="shared" ca="1" si="123"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="DY37" s="4" t="str">
         <f t="shared" ca="1" si="135"/>
@@ -25355,7 +25356,7 @@
       </c>
       <c r="EB37" s="4">
         <f t="shared" ca="1" si="138"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="EC37" s="4" t="str">
         <f t="shared" ca="1" si="139"/>
@@ -25379,7 +25380,7 @@
       </c>
       <c r="EH37" s="4">
         <f t="shared" ca="1" si="144"/>
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="EI37" s="4" t="str">
         <f t="shared" ca="1" si="164"/>
@@ -25559,7 +25560,7 @@
       </c>
       <c r="GB37" s="5">
         <f t="shared" si="124"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="GC37" s="6" t="e">
         <f t="shared" ca="1" si="125"/>
@@ -25587,7 +25588,7 @@
       </c>
       <c r="GI37" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="GJ37" s="5" t="e">
         <f t="shared" si="132"/>
@@ -25632,31 +25633,31 @@
       </c>
       <c r="M38" s="8">
         <f t="shared" si="89"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N38" s="8">
         <f t="shared" si="90"/>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O38" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="P38" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="Q38" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T38" s="4">
         <f t="shared" si="94"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="U38" s="4">
         <f t="shared" si="95"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V38" s="4">
         <f t="shared" si="96"/>
@@ -26080,7 +26081,7 @@
       </c>
       <c r="DX38" s="4">
         <f t="shared" ca="1" si="123"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="DY38" s="4" t="str">
         <f t="shared" ca="1" si="135"/>
@@ -26136,7 +26137,7 @@
       </c>
       <c r="EL38" s="4">
         <f t="shared" ca="1" si="145"/>
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="EM38" s="4" t="str">
         <f t="shared" ca="1" si="146"/>
@@ -26300,35 +26301,35 @@
       </c>
       <c r="GB38" s="5">
         <f t="shared" si="124"/>
-        <v>37</v>
-      </c>
-      <c r="GC38" s="6" t="e">
+        <v>35</v>
+      </c>
+      <c r="GC38" s="6">
         <f t="shared" ca="1" si="125"/>
+        <v>5</v>
+      </c>
+      <c r="GD38" s="6">
+        <f t="shared" ca="1" si="126"/>
+        <v>0</v>
+      </c>
+      <c r="GE38" s="6">
+        <f t="shared" ca="1" si="127"/>
+        <v>0</v>
+      </c>
+      <c r="GF38" s="6" t="e">
+        <f t="shared" ca="1" si="128"/>
         <v>#N/A</v>
       </c>
-      <c r="GD38" s="6" t="e">
-        <f t="shared" ca="1" si="126"/>
+      <c r="GG38" s="6" t="e">
+        <f t="shared" ca="1" si="129"/>
         <v>#N/A</v>
       </c>
-      <c r="GE38" s="6" t="e">
-        <f t="shared" ca="1" si="127"/>
+      <c r="GH38" s="6" t="e">
+        <f t="shared" ca="1" si="130"/>
         <v>#N/A</v>
-      </c>
-      <c r="GF38" s="6">
-        <f t="shared" ca="1" si="128"/>
-        <v>5</v>
-      </c>
-      <c r="GG38" s="6">
-        <f t="shared" ca="1" si="129"/>
-        <v>0</v>
-      </c>
-      <c r="GH38" s="6">
-        <f t="shared" ca="1" si="130"/>
-        <v>0</v>
       </c>
       <c r="GI38" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="GJ38" s="5" t="e">
         <f t="shared" si="132"/>
@@ -27833,19 +27834,19 @@
       </c>
       <c r="M41" s="8">
         <f t="shared" si="89"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="N41" s="8">
         <f t="shared" si="90"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="O41" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="P41" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="Q41" s="8">
         <f t="shared" ca="1" si="93"/>
@@ -27853,11 +27854,11 @@
       </c>
       <c r="T41" s="4">
         <f t="shared" si="94"/>
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="U41" s="4">
         <f t="shared" si="95"/>
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="V41" s="4">
         <f t="shared" si="96"/>
@@ -27869,11 +27870,11 @@
       </c>
       <c r="X41" s="4">
         <f t="shared" si="98"/>
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="Y41" s="4">
         <f t="shared" si="99"/>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="AA41" s="4" t="str">
         <f t="shared" ca="1" si="190"/>
@@ -28401,7 +28402,7 @@
       </c>
       <c r="FB41" s="4">
         <f t="shared" ca="1" si="161"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="FC41" s="4" t="str">
         <f t="shared" ca="1" si="162"/>
@@ -28501,7 +28502,7 @@
       </c>
       <c r="GB41" s="5">
         <f t="shared" si="124"/>
-        <v>59.75</v>
+        <v>47.75</v>
       </c>
       <c r="GC41" s="6" t="e">
         <f t="shared" si="125"/>
@@ -28533,7 +28534,7 @@
       </c>
       <c r="GJ41" s="5">
         <f t="shared" si="132"/>
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="42" spans="1:192" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -28570,31 +28571,31 @@
       </c>
       <c r="M42" s="8">
         <f t="shared" si="89"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="N42" s="8">
         <f t="shared" si="90"/>
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="O42" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="P42" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="Q42" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="T42" s="4">
         <f t="shared" si="94"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="U42" s="4">
         <f t="shared" si="95"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="V42" s="4">
         <f t="shared" si="96"/>
@@ -29054,7 +29055,7 @@
       </c>
       <c r="EG42" s="4">
         <f t="shared" ca="1" si="143"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="EH42" s="4" t="str">
         <f t="shared" ca="1" si="144"/>
@@ -29238,7 +29239,7 @@
       </c>
       <c r="GB42" s="5">
         <f t="shared" si="124"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="GC42" s="6" t="e">
         <f t="shared" ca="1" si="125"/>
@@ -29266,7 +29267,7 @@
       </c>
       <c r="GI42" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="GJ42" s="5" t="e">
         <f t="shared" si="132"/>
@@ -29307,31 +29308,31 @@
       </c>
       <c r="M43" s="8">
         <f t="shared" si="89"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="N43" s="8">
         <f t="shared" si="90"/>
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="O43" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="P43" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="Q43" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="T43" s="4">
         <f t="shared" si="94"/>
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U43" s="4">
         <f t="shared" si="95"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="V43" s="4">
         <f t="shared" si="96"/>
@@ -29791,7 +29792,7 @@
       </c>
       <c r="EG43" s="4">
         <f t="shared" ca="1" si="143"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="EH43" s="4" t="str">
         <f t="shared" ca="1" si="144"/>
@@ -29975,7 +29976,7 @@
       </c>
       <c r="GB43" s="5">
         <f t="shared" si="124"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="GC43" s="6" t="e">
         <f t="shared" ca="1" si="125"/>
@@ -30003,7 +30004,7 @@
       </c>
       <c r="GI43" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="GJ43" s="5" t="e">
         <f t="shared" si="132"/>
@@ -30048,15 +30049,15 @@
       </c>
       <c r="O44" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="P44" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="Q44" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="T44" s="4">
         <f t="shared" si="94"/>
@@ -30524,7 +30525,7 @@
       </c>
       <c r="EG44" s="4">
         <f t="shared" ca="1" si="143"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="EH44" s="4" t="str">
         <f t="shared" ca="1" si="144"/>
@@ -30736,7 +30737,7 @@
       </c>
       <c r="GI44" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="GJ44" s="5" t="e">
         <f t="shared" si="132"/>
@@ -30781,15 +30782,15 @@
       </c>
       <c r="O45" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="P45" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="Q45" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="T45" s="4">
         <f t="shared" si="94"/>
@@ -31257,7 +31258,7 @@
       </c>
       <c r="EG45" s="4">
         <f t="shared" ca="1" si="143"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="EH45" s="4" t="str">
         <f t="shared" ca="1" si="144"/>
@@ -31469,7 +31470,7 @@
       </c>
       <c r="GI45" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="GJ45" s="5" t="e">
         <f t="shared" si="132"/>
@@ -31510,31 +31511,31 @@
       </c>
       <c r="M46" s="8">
         <f t="shared" si="89"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="N46" s="8">
         <f t="shared" si="90"/>
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="O46" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="P46" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="Q46" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="T46" s="4">
         <f t="shared" si="94"/>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="U46" s="4">
         <f t="shared" si="95"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="V46" s="4">
         <f t="shared" si="96"/>
@@ -31994,7 +31995,7 @@
       </c>
       <c r="EG46" s="4">
         <f t="shared" ca="1" si="143"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="EH46" s="4" t="str">
         <f t="shared" ca="1" si="144"/>
@@ -32178,35 +32179,35 @@
       </c>
       <c r="GB46" s="5">
         <f t="shared" si="124"/>
-        <v>45</v>
-      </c>
-      <c r="GC46" s="6" t="e">
+        <v>40</v>
+      </c>
+      <c r="GC46" s="6">
         <f t="shared" ca="1" si="125"/>
+        <v>8</v>
+      </c>
+      <c r="GD46" s="6">
+        <f t="shared" ca="1" si="126"/>
+        <v>0</v>
+      </c>
+      <c r="GE46" s="6">
+        <f t="shared" ca="1" si="127"/>
+        <v>0</v>
+      </c>
+      <c r="GF46" s="6" t="e">
+        <f t="shared" ca="1" si="128"/>
         <v>#N/A</v>
       </c>
-      <c r="GD46" s="6" t="e">
-        <f t="shared" ca="1" si="126"/>
+      <c r="GG46" s="6" t="e">
+        <f t="shared" ca="1" si="129"/>
         <v>#N/A</v>
       </c>
-      <c r="GE46" s="6" t="e">
-        <f t="shared" ca="1" si="127"/>
+      <c r="GH46" s="6" t="e">
+        <f t="shared" ca="1" si="130"/>
         <v>#N/A</v>
-      </c>
-      <c r="GF46" s="6">
-        <f t="shared" ca="1" si="128"/>
-        <v>8</v>
-      </c>
-      <c r="GG46" s="6">
-        <f t="shared" ca="1" si="129"/>
-        <v>0</v>
-      </c>
-      <c r="GH46" s="6">
-        <f t="shared" ca="1" si="130"/>
-        <v>0</v>
       </c>
       <c r="GI46" s="5">
         <f t="shared" ca="1" si="131"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="GJ46" s="5" t="e">
         <f t="shared" si="132"/>
@@ -35875,18 +35876,16 @@
       <c r="H52" s="17"/>
       <c r="I52" s="23">
         <f t="shared" si="61"/>
-        <v>15</v>
-      </c>
-      <c r="J52" s="16">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J52" s="16"/>
       <c r="K52" s="16">
         <f t="shared" si="59"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L52" s="8">
         <f t="shared" si="88"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M52" s="8">
         <f t="shared" si="89"/>
@@ -35894,19 +35893,19 @@
       </c>
       <c r="N52" s="8">
         <f t="shared" si="90"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="O52" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P52" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q52" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="T52" s="4">
         <f t="shared" si="94"/>
@@ -36250,7 +36249,7 @@
       </c>
       <c r="DB52" s="4">
         <f t="shared" ca="1" si="101"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="DC52" s="4" t="str">
         <f t="shared" ca="1" si="102"/>
@@ -36422,7 +36421,7 @@
       </c>
       <c r="ES52" s="4">
         <f t="shared" ca="1" si="152"/>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="ET52" s="4" t="str">
         <f t="shared" ca="1" si="153"/>
@@ -36558,39 +36557,39 @@
       </c>
       <c r="GB52" s="5">
         <f t="shared" si="124"/>
-        <v>0</v>
-      </c>
-      <c r="GC52" s="6">
-        <f t="shared" ca="1" si="125"/>
-        <v>15</v>
-      </c>
-      <c r="GD52" s="6">
-        <f t="shared" ca="1" si="126"/>
-        <v>0</v>
-      </c>
-      <c r="GE52" s="6">
-        <f t="shared" ca="1" si="127"/>
-        <v>0</v>
+        <v>-0.25</v>
+      </c>
+      <c r="GC52" s="6" t="e">
+        <f t="shared" si="125"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GD52" s="6" t="e">
+        <f t="shared" si="126"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GE52" s="6" t="e">
+        <f t="shared" si="127"/>
+        <v>#N/A</v>
       </c>
       <c r="GF52" s="6" t="e">
-        <f t="shared" ca="1" si="128"/>
+        <f t="shared" si="128"/>
         <v>#N/A</v>
       </c>
       <c r="GG52" s="6" t="e">
-        <f t="shared" ca="1" si="129"/>
+        <f t="shared" si="129"/>
         <v>#N/A</v>
       </c>
       <c r="GH52" s="6" t="e">
-        <f t="shared" ca="1" si="130"/>
+        <f t="shared" si="130"/>
         <v>#N/A</v>
       </c>
-      <c r="GI52" s="5">
-        <f t="shared" ca="1" si="131"/>
-        <v>0</v>
-      </c>
-      <c r="GJ52" s="5" t="e">
+      <c r="GI52" s="5" t="e">
+        <f t="shared" si="131"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GJ52" s="5">
         <f t="shared" si="132"/>
-        <v>#N/A</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="53" spans="1:192" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -36612,46 +36611,44 @@
       <c r="H53" s="17"/>
       <c r="I53" s="23">
         <f t="shared" si="61"/>
-        <v>15</v>
-      </c>
-      <c r="J53" s="16">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J53" s="16"/>
       <c r="K53" s="16">
         <f t="shared" si="59"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L53" s="8">
         <f t="shared" si="88"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M53" s="8">
         <f t="shared" si="89"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N53" s="8">
         <f t="shared" si="90"/>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="O53" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="P53" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q53" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="T53" s="4">
         <f t="shared" si="94"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="U53" s="4">
         <f t="shared" si="95"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V53" s="4">
         <f t="shared" si="96"/>
@@ -37027,7 +37024,7 @@
       </c>
       <c r="DL53" s="4">
         <f t="shared" ca="1" si="111"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="DM53" s="4" t="str">
         <f t="shared" ca="1" si="112"/>
@@ -37163,7 +37160,7 @@
       </c>
       <c r="ET53" s="4">
         <f t="shared" ca="1" si="153"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="EU53" s="4" t="str">
         <f t="shared" ca="1" si="154"/>
@@ -37295,39 +37292,39 @@
       </c>
       <c r="GB53" s="5">
         <f t="shared" si="124"/>
-        <v>15</v>
-      </c>
-      <c r="GC53" s="6">
-        <f t="shared" ca="1" si="125"/>
-        <v>15</v>
-      </c>
-      <c r="GD53" s="6">
-        <f t="shared" ca="1" si="126"/>
-        <v>0</v>
-      </c>
-      <c r="GE53" s="6">
-        <f t="shared" ca="1" si="127"/>
-        <v>0</v>
+        <v>13.75</v>
+      </c>
+      <c r="GC53" s="6" t="e">
+        <f t="shared" si="125"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GD53" s="6" t="e">
+        <f t="shared" si="126"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GE53" s="6" t="e">
+        <f t="shared" si="127"/>
+        <v>#N/A</v>
       </c>
       <c r="GF53" s="6" t="e">
-        <f t="shared" ca="1" si="128"/>
+        <f t="shared" si="128"/>
         <v>#N/A</v>
       </c>
       <c r="GG53" s="6" t="e">
-        <f t="shared" ca="1" si="129"/>
+        <f t="shared" si="129"/>
         <v>#N/A</v>
       </c>
       <c r="GH53" s="6" t="e">
-        <f t="shared" ca="1" si="130"/>
+        <f t="shared" si="130"/>
         <v>#N/A</v>
       </c>
-      <c r="GI53" s="5">
-        <f t="shared" ca="1" si="131"/>
-        <v>0</v>
-      </c>
-      <c r="GJ53" s="5" t="e">
+      <c r="GI53" s="5" t="e">
+        <f t="shared" si="131"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GJ53" s="5">
         <f t="shared" si="132"/>
-        <v>#N/A</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="54" spans="1:192" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -37349,46 +37346,44 @@
       <c r="H54" s="17"/>
       <c r="I54" s="23">
         <f t="shared" si="61"/>
-        <v>15</v>
-      </c>
-      <c r="J54" s="16">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J54" s="16"/>
       <c r="K54" s="16">
         <f t="shared" si="59"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L54" s="8">
         <f t="shared" si="88"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M54" s="8">
         <f t="shared" si="89"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N54" s="8">
         <f t="shared" si="90"/>
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="O54" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="P54" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="Q54" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="T54" s="4">
         <f t="shared" si="94"/>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="U54" s="4">
         <f t="shared" si="95"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V54" s="4">
         <f t="shared" si="96"/>
@@ -37812,7 +37807,7 @@
       </c>
       <c r="DX54" s="4">
         <f t="shared" ca="1" si="123"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="DY54" s="4" t="str">
         <f t="shared" ca="1" si="135"/>
@@ -37904,7 +37899,7 @@
       </c>
       <c r="EU54" s="4">
         <f t="shared" ca="1" si="154"/>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="EV54" s="4" t="str">
         <f t="shared" ca="1" si="155"/>
@@ -38032,39 +38027,39 @@
       </c>
       <c r="GB54" s="5">
         <f t="shared" si="124"/>
-        <v>30</v>
-      </c>
-      <c r="GC54" s="6">
-        <f t="shared" ca="1" si="125"/>
-        <v>15</v>
-      </c>
-      <c r="GD54" s="6">
-        <f t="shared" ca="1" si="126"/>
-        <v>0</v>
-      </c>
-      <c r="GE54" s="6">
-        <f t="shared" ca="1" si="127"/>
-        <v>0</v>
+        <v>27.75</v>
+      </c>
+      <c r="GC54" s="6" t="e">
+        <f t="shared" si="125"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GD54" s="6" t="e">
+        <f t="shared" si="126"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GE54" s="6" t="e">
+        <f t="shared" si="127"/>
+        <v>#N/A</v>
       </c>
       <c r="GF54" s="6" t="e">
-        <f t="shared" ca="1" si="128"/>
+        <f t="shared" si="128"/>
         <v>#N/A</v>
       </c>
       <c r="GG54" s="6" t="e">
-        <f t="shared" ca="1" si="129"/>
+        <f t="shared" si="129"/>
         <v>#N/A</v>
       </c>
       <c r="GH54" s="6" t="e">
-        <f t="shared" ca="1" si="130"/>
+        <f t="shared" si="130"/>
         <v>#N/A</v>
       </c>
-      <c r="GI54" s="5">
-        <f t="shared" ca="1" si="131"/>
-        <v>0</v>
-      </c>
-      <c r="GJ54" s="5" t="e">
+      <c r="GI54" s="5" t="e">
+        <f t="shared" si="131"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GJ54" s="5">
         <f t="shared" si="132"/>
-        <v>#N/A</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="55" spans="1:192" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -38086,46 +38081,44 @@
       <c r="H55" s="17"/>
       <c r="I55" s="23">
         <f t="shared" si="61"/>
-        <v>15</v>
-      </c>
-      <c r="J55" s="16">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J55" s="16"/>
       <c r="K55" s="16">
         <f t="shared" si="59"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L55" s="8">
         <f t="shared" si="88"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M55" s="8">
         <f t="shared" si="89"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="N55" s="8">
         <f t="shared" si="90"/>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="O55" s="8">
         <f t="shared" ca="1" si="91"/>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="P55" s="8">
         <f t="shared" ca="1" si="92"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="Q55" s="8">
         <f t="shared" ca="1" si="93"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T55" s="4">
         <f t="shared" si="94"/>
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="U55" s="4">
         <f t="shared" si="95"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="V55" s="4">
         <f t="shared" si="96"/>
@@ -38585,7 +38578,7 @@
       </c>
       <c r="EG55" s="4">
         <f t="shared" ca="1" si="143"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="EH55" s="4" t="str">
         <f t="shared" ca="1" si="144"/>
@@ -38769,39 +38762,39 @@
       </c>
       <c r="GB55" s="5">
         <f t="shared" si="124"/>
-        <v>45</v>
-      </c>
-      <c r="GC55" s="6">
-        <f t="shared" ca="1" si="125"/>
-        <v>15</v>
-      </c>
-      <c r="GD55" s="6">
-        <f t="shared" ca="1" si="126"/>
-        <v>0</v>
-      </c>
-      <c r="GE55" s="6">
-        <f t="shared" ca="1" si="127"/>
-        <v>0</v>
+        <v>39.75</v>
+      </c>
+      <c r="GC55" s="6" t="e">
+        <f t="shared" si="125"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GD55" s="6" t="e">
+        <f t="shared" si="126"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GE55" s="6" t="e">
+        <f t="shared" si="127"/>
+        <v>#N/A</v>
       </c>
       <c r="GF55" s="6" t="e">
-        <f t="shared" ca="1" si="128"/>
+        <f t="shared" si="128"/>
         <v>#N/A</v>
       </c>
       <c r="GG55" s="6" t="e">
-        <f t="shared" ca="1" si="129"/>
+        <f t="shared" si="129"/>
         <v>#N/A</v>
       </c>
       <c r="GH55" s="6" t="e">
-        <f t="shared" ca="1" si="130"/>
+        <f t="shared" si="130"/>
         <v>#N/A</v>
       </c>
-      <c r="GI55" s="5">
-        <f t="shared" ca="1" si="131"/>
-        <v>0</v>
-      </c>
-      <c r="GJ55" s="5" t="e">
+      <c r="GI55" s="5" t="e">
+        <f t="shared" si="131"/>
+        <v>#N/A</v>
+      </c>
+      <c r="GJ55" s="5">
         <f t="shared" si="132"/>
-        <v>#N/A</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="56" spans="1:192" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -43190,19 +43183,19 @@
       </c>
       <c r="M62" s="8">
         <f t="shared" si="56"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="N62" s="8">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="O62" s="8">
         <f t="shared" si="57"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="P62" s="9">
         <f>N62</f>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="Q62" s="8">
         <f t="shared" si="58"/>
@@ -43210,19 +43203,19 @@
       </c>
       <c r="T62" s="4">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U62" s="4">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V62" s="4">
         <f t="shared" si="5"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="W62" s="4">
         <f t="shared" si="6"/>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="X62" s="4">
         <f t="shared" si="7"/>
@@ -43858,7 +43851,7 @@
       </c>
       <c r="GB62" s="5">
         <f>IF(B62="",NA(),IF(L62=0,M62-0.25,M62))</f>
-        <v>59.75</v>
+        <v>47.75</v>
       </c>
       <c r="GC62" s="6" t="e">
         <f>IF(B62="",NA(),IF(L62=0,NA(),IF(Q62&lt;=0.01,L62,NA())))</f>
@@ -43890,7 +43883,7 @@
       </c>
       <c r="GJ62" s="5">
         <f>IF(B62="",NA(),IF(L62=0,$M$62/40,NA()))</f>
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="63" spans="1:192" ht="15" x14ac:dyDescent="0.2">
@@ -43931,7 +43924,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Beta, Triangular"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>